<commit_message>
add biomass macrofauna composition analysis
</commit_message>
<xml_diff>
--- a/table/biomass_permanova.xlsx
+++ b/table/biomass_permanova.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,37 +390,54 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.583988084513391</v>
+        <v>0.8740278822251073</v>
       </c>
       <c r="C2">
-        <v>0.04686598528541525</v>
+        <v>0.06870153376771632</v>
       </c>
       <c r="D2">
-        <v>1.524282547279488</v>
+        <v>2.922387458680074</v>
       </c>
       <c r="E2">
-        <v>0.08943</v>
+        <v>0.01346</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>11.8768207719928</v>
+        <v>5.268311750865272</v>
       </c>
       <c r="C3">
-        <v>0.9531340147145848</v>
+        <v>0.4141070382440141</v>
+      </c>
+      <c r="D3">
+        <v>1.957228202676015</v>
+      </c>
+      <c r="E3">
+        <v>0.00132</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>6.579761814895401</v>
+      </c>
+      <c r="C4">
+        <v>0.51719142798827</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
         <v>32</v>
       </c>
-      <c r="B4">
-        <v>12.46080885650619</v>
-      </c>
-      <c r="C4">
+      <c r="B5">
+        <v>12.72210144798578</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
     </row>
@@ -474,19 +491,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.02878732565577795</v>
+        <v>2.994149613517597e-005</v>
       </c>
       <c r="C2">
-        <v>0.02878732565577795</v>
+        <v>2.994149613517597e-005</v>
       </c>
       <c r="D2">
-        <v>2.804404365325029</v>
+        <v>0.001278238776438813</v>
       </c>
       <c r="E2">
         <v>999</v>
       </c>
       <c r="F2">
-        <v>0.111</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="3">
@@ -494,10 +511,10 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>0.3182162695092249</v>
+        <v>0.7261447526857168</v>
       </c>
       <c r="C3">
-        <v>0.01026504095191048</v>
+        <v>0.02342402428018441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>